<commit_message>
This is a partially working queue. I am going to implement modular arithmetics as it seems to be the easiest solution.
</commit_message>
<xml_diff>
--- a/AlgTut1exercise2/testColouring.xlsx
+++ b/AlgTut1exercise2/testColouring.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benwo\Documents\GitHub\COMP1201\AlgTut1exercise2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A16087-3D5A-4E5D-97AC-C64F90B18BE1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8339733-F9AB-4233-B852-8B3EC3B70C80}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Java Books" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -481,6 +481,45 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0">
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t> complexity of the Graph-Colouring problem</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -558,8 +597,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.17210410027152892"/>
-                  <c:y val="9.1274203277194321E-2"/>
+                  <c:x val="-5.9595940229774602E-2"/>
+                  <c:y val="8.9534918345903686E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -575,16 +614,16 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
                           <a:lumOff val="35000"/>
                         </a:schemeClr>
                       </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     </a:defRPr>
                   </a:pPr>
                   <a:endParaRPr lang="en-US"/>
@@ -685,6 +724,82 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> of Nodes </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" i="1" baseline="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>N</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" sz="1400" i="1">
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -747,6 +862,113 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" i="1">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>f</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>(</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" i="1">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>): Time (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" i="1">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>in Log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" i="1" baseline="-25000">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400" i="1">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>(seconds)</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1400">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -778,7 +1000,7 @@
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -835,7 +1057,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1992,16 +2214,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>166686</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>185736</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142876</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2328,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>